<commit_message>
introduction small changes, table
</commit_message>
<xml_diff>
--- a/figures/table1-lat-gradients.xlsx
+++ b/figures/table1-lat-gradients.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\PalaeoClimateGradient\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FA40C5-E0E1-4F3D-BE2E-0C2EDD7CE780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68316895-F391-4044-BD1C-312C747354F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4788" yWindow="2820" windowWidth="17280" windowHeight="8880" xr2:uid="{AF86497D-FCFA-4759-A7D9-E276B06DBA8C}"/>
+    <workbookView xWindow="28680" yWindow="-5580" windowWidth="29040" windowHeight="15840" xr2:uid="{AF86497D-FCFA-4759-A7D9-E276B06DBA8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>Source</t>
   </si>
@@ -71,9 +71,6 @@
     <t>equator - polar circle</t>
   </si>
   <si>
-    <t>Tex, Uk37</t>
-  </si>
-  <si>
     <t>comment</t>
   </si>
   <si>
@@ -92,16 +89,49 @@
     <t>13 (11, 14)</t>
   </si>
   <si>
-    <t>Tex, MBT, clumped, Mg/Ca, d18O</t>
-  </si>
-  <si>
     <t>EECO</t>
   </si>
   <si>
-    <t>Keating-Bitoni et al 2011</t>
-  </si>
-  <si>
-    <t>Bij et al 2009</t>
+    <t>Evans et al. 2018</t>
+  </si>
+  <si>
+    <t>Keating-Bitoni et al. 2011</t>
+  </si>
+  <si>
+    <t>Bij et al. 2009</t>
+  </si>
+  <si>
+    <t>clumped, deep-water Mg/Ca</t>
+  </si>
+  <si>
+    <t>mainly non-EECO data</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>Tierney et al. 2017</t>
+  </si>
+  <si>
+    <t>TEX86</t>
+  </si>
+  <si>
+    <t>TEX86, MBT, clumped, Mg/Ca, d18O</t>
+  </si>
+  <si>
+    <t>TEX86, Uk37</t>
+  </si>
+  <si>
+    <t>Gaussian function</t>
+  </si>
+  <si>
+    <t>Cramwinckel et al. 2018</t>
+  </si>
+  <si>
+    <t>equator - deep water</t>
+  </si>
+  <si>
+    <t>TEX86, clumped, Mg/Ca, d18O, deepwater d18O</t>
   </si>
 </sst>
 </file>
@@ -137,8 +167,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,7 +478,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -453,26 +486,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1CE2AB0-960D-46B3-8696-355F1D96B056}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection sqref="A1:I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" customWidth="1"/>
-    <col min="4" max="4" width="36.88671875" customWidth="1"/>
-    <col min="5" max="5" width="5.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" customWidth="1"/>
-    <col min="7" max="7" width="19.88671875" customWidth="1"/>
-    <col min="8" max="8" width="27.88671875" customWidth="1"/>
-    <col min="9" max="9" width="25.21875" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="46.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" customWidth="1"/>
+    <col min="9" max="9" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -492,18 +525,18 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -512,7 +545,7 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -521,27 +554,27 @@
         <v>10</v>
       </c>
       <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -550,10 +583,91 @@
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1">
+        <v>21</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1">
+        <v>20</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>